<commit_message>
BEFORE NEW FORUM APP
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VS\Carpetas\Entrega_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283C4601-51BC-4494-8670-684D37AA4995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30230596-FAD0-4D43-9D17-22612FF0346E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
   <si>
     <t>Problema</t>
   </si>
@@ -115,6 +115,31 @@
   </si>
   <si>
     <t>ABCDE4848145105187166120139731921871871674729681652003412086271041211291121057812302017613720020012036211601618941152144</t>
+  </si>
+  <si>
+    <t>IntegrityError at /users/register_view/
+UNIQUE constraint failed: auth_user.username</t>
+  </si>
+  <si>
+    <t>from django.contrib.auth.models import User
+if User.objects.filter(username=username).exists():
+    # Manejar el caso en el que el nombre de usuario ya existe</t>
+  </si>
+  <si>
+    <t>Se escribe un usuario que ya existe</t>
+  </si>
+  <si>
+    <t>from django import forms
+from django.contrib.auth.models import User
+class UserRegistrationForm(forms.ModelForm):
+    class Meta:
+        model = User
+        fields = ['username', 'password']
+    def clean_username(self):
+        username = self.cleaned_data.get('username')
+        if User.objects.filter(username=username).exists():
+            raise forms.ValidationError("El nombre de usuario ya está en uso.")
+        return username</t>
   </si>
 </sst>
 </file>
@@ -153,7 +178,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +470,7 @@
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,15 +481,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -472,23 +497,37 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -765,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B8C083-2DDA-41FF-AACC-B226B5DD11AF}">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Q50" sqref="Q50"/>
     </sheetView>
   </sheetViews>

</xml_diff>